<commit_message>
add all the rest of the genes
</commit_message>
<xml_diff>
--- a/src/cellphonedb/summary/simple_significant_interactions_60_with_genes.xlsx
+++ b/src/cellphonedb/summary/simple_significant_interactions_60_with_genes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Imm.DAM.0" sheetId="1" state="visible" r:id="rId2"/>
@@ -1025,7 +1025,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.05"/>
@@ -1277,7 +1277,7 @@
       <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.34"/>
@@ -1898,11 +1898,11 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.24"/>
@@ -2609,10 +2609,10 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.24"/>
@@ -3084,7 +3084,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.35"/>
@@ -3366,7 +3366,7 @@
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.35"/>
@@ -3816,7 +3816,7 @@
       <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.35"/>
@@ -4280,11 +4280,11 @@
   </sheetPr>
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.35"/>
@@ -4514,7 +4514,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>43</v>
       </c>

</xml_diff>